<commit_message>
AI phân tích báo giá excel
</commit_message>
<xml_diff>
--- a/20251115. Anh Tượng Tân Phú.xlsx
+++ b/20251115. Anh Tượng Tân Phú.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1. PhucDatdoor\1. PHUCDATDOOR\3. PHÚC ĐẠT DOOR\02. BẢNG BÁO GIÁ\NĂM 2025\391.20251115.  Anh Tượng Tân Phú\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Financial-management-Phuc-Dat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4347F5E3-D050-43EE-B4C1-90CD61A198CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9180" tabRatio="599" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="599" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" state="hidden" r:id="rId1"/>
@@ -27,7 +28,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet2!$A$1:$K$15</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">XFNK!$B$1:$M$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1026,7 +1027,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1411,7 +1412,7 @@
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1537,320 +1538,269 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1882,7 +1832,7 @@
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="16"/>
+    <cellStyle name="Comma 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -1896,12 +1846,12 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="17"/>
-    <cellStyle name="Normal 3" xfId="18"/>
-    <cellStyle name="Normal 4" xfId="15"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 4" xfId="15" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Percent" xfId="20" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="19"/>
+    <cellStyle name="Percent 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2093,7 +2043,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2186,7 +2142,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2224,7 +2186,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2262,7 +2230,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2300,7 +2274,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2338,7 +2318,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2660,7 +2646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2670,153 +2656,153 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="4.88671875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="4.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="103.5" customHeight="1">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="2:12" ht="54.75" customHeight="1">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-    </row>
-    <row r="6" spans="2:12" ht="16.8">
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="2:12" ht="16.5">
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="16.8">
-      <c r="C7" s="79" t="s">
+    <row r="7" spans="2:12" ht="16.5">
+      <c r="C7" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="2:12" ht="15.6">
-      <c r="B8" s="80" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+    </row>
+    <row r="8" spans="2:12" ht="15.75">
+      <c r="B8" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83" t="s">
+      <c r="F8" s="69"/>
+      <c r="G8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="71" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="33.75" customHeight="1">
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="85"/>
-    </row>
-    <row r="10" spans="2:12" ht="93.6">
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
+    </row>
+    <row r="10" spans="2:12" ht="94.5">
       <c r="B10" s="5">
         <v>1</v>
       </c>
@@ -2840,7 +2826,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="2:12" ht="93.6">
+    <row r="11" spans="2:12" ht="94.5">
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -2865,7 +2851,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="2:12" ht="93.6">
+    <row r="12" spans="2:12" ht="94.5">
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -2889,7 +2875,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="2:12" ht="93.6">
+    <row r="13" spans="2:12" ht="94.5">
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -2913,7 +2899,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="2:12" ht="93.6">
+    <row r="14" spans="2:12" ht="94.5">
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -2937,17 +2923,17 @@
       <c r="J14" s="8"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="2:12" s="12" customFormat="1" ht="15.6">
+    <row r="15" spans="2:12" s="12" customFormat="1" ht="15.75">
       <c r="B15" s="14"/>
-      <c r="C15" s="72" t="s">
+      <c r="C15" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="74"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
       <c r="J15" s="4">
         <f>SUM(J11:J11)</f>
         <v>0</v>
@@ -3134,7 +3120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3144,153 +3130,153 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="4.88671875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="4.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="108" customHeight="1">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
     </row>
     <row r="2" spans="2:11" ht="49.5" customHeight="1">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-    </row>
-    <row r="6" spans="2:11" ht="16.8">
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="2:11" ht="16.5">
       <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="16.8">
-      <c r="C7" s="79" t="s">
+    <row r="7" spans="2:11" ht="16.5">
+      <c r="C7" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="2:11" ht="15.6">
-      <c r="B8" s="80" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+    </row>
+    <row r="8" spans="2:11" ht="15.75">
+      <c r="B8" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83" t="s">
+      <c r="F8" s="69"/>
+      <c r="G8" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="31.2">
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
+    <row r="9" spans="2:11" ht="31.5">
+      <c r="B9" s="66"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="13" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="85"/>
-    </row>
-    <row r="10" spans="2:11" ht="93.6">
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
+    </row>
+    <row r="10" spans="2:11" ht="94.5">
       <c r="B10" s="5">
         <v>1</v>
       </c>
@@ -3314,7 +3300,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="2:11" ht="93.6">
+    <row r="11" spans="2:11" ht="94.5">
       <c r="B11" s="5">
         <v>2</v>
       </c>
@@ -3338,7 +3324,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="2:11" ht="93.6">
+    <row r="12" spans="2:11" ht="94.5">
       <c r="B12" s="5">
         <v>3</v>
       </c>
@@ -3362,7 +3348,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="2:11" ht="93.6">
+    <row r="13" spans="2:11" ht="94.5">
       <c r="B13" s="5">
         <v>4</v>
       </c>
@@ -3386,7 +3372,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="2:11" ht="62.4">
+    <row r="14" spans="2:11" ht="63">
       <c r="B14" s="5">
         <v>5</v>
       </c>
@@ -3410,7 +3396,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="2:11" ht="46.8">
+    <row r="15" spans="2:11" ht="47.25">
       <c r="B15" s="5">
         <v>6</v>
       </c>
@@ -3434,7 +3420,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="2:11" ht="15.6">
+    <row r="16" spans="2:11" ht="15.75">
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -3458,7 +3444,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="2:12" ht="31.2">
+    <row r="17" spans="2:12" ht="31.5">
       <c r="B17" s="5">
         <v>8</v>
       </c>
@@ -3482,7 +3468,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="2:12" ht="15.6">
+    <row r="18" spans="2:12" ht="31.5">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -3506,17 +3492,17 @@
       <c r="J18" s="8"/>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="2:12" s="12" customFormat="1" ht="15.6">
+    <row r="19" spans="2:12" s="12" customFormat="1" ht="15.75">
       <c r="B19" s="14"/>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="74"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
       <c r="J19" s="4" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
@@ -3526,15 +3512,15 @@
     </row>
     <row r="20" spans="2:12" s="12" customFormat="1" ht="48.75" customHeight="1">
       <c r="B20" s="14"/>
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="74"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="60"/>
       <c r="J20" s="4" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
@@ -3543,17 +3529,17 @@
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="2:12" s="12" customFormat="1" ht="87" customHeight="1">
-      <c r="B21" s="86" t="s">
+      <c r="B21" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="2:12" s="12" customFormat="1">
@@ -3690,12 +3676,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="C19:I19"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="C3:K5"/>
@@ -3706,6 +3686,12 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="C19:I19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3715,39 +3701,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A6:F24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:6">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="87"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="18" t="s">
@@ -4081,241 +4067,241 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="4.88671875" style="68" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="68" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" style="68" customWidth="1"/>
-    <col min="5" max="5" width="46.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="71" customWidth="1"/>
-    <col min="13" max="13" width="24.109375" style="68" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" style="71" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="4.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="112.5" customHeight="1">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="2:15" ht="49.5" customHeight="1">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-    </row>
-    <row r="3" spans="2:15" ht="13.95" customHeight="1">
-      <c r="B3" s="78" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+    </row>
+    <row r="3" spans="2:15" ht="13.9" customHeight="1">
+      <c r="B3" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-    </row>
-    <row r="6" spans="2:15" ht="16.8">
-      <c r="B6" s="110" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+    </row>
+    <row r="6" spans="2:15" ht="16.5">
+      <c r="B6" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="M6" s="111"/>
-    </row>
-    <row r="7" spans="2:15" ht="16.8">
-      <c r="B7" s="94" t="s">
+      <c r="M6" s="98"/>
+    </row>
+    <row r="7" spans="2:15" ht="16.5">
+      <c r="B7" s="87" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="71" t="s">
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="95" t="s">
+      <c r="L7" s="88" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="95"/>
+      <c r="M7" s="88"/>
     </row>
     <row r="8" spans="2:15" ht="33.6" customHeight="1">
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="106" t="s">
+      <c r="E9" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="108" t="s">
+      <c r="F9" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="104" t="s">
+      <c r="G9" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="105"/>
-      <c r="I9" s="96" t="s">
+      <c r="H9" s="96"/>
+      <c r="I9" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="96" t="s">
+      <c r="J9" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="96" t="s">
+      <c r="K9" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="98" t="s">
+      <c r="L9" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="100" t="s">
+      <c r="M9" s="81" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="30" customHeight="1">
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="70" t="s">
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="70" t="s">
+      <c r="H10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="101"/>
-    </row>
-    <row r="11" spans="2:15" s="47" customFormat="1" ht="202.8">
-      <c r="B11" s="88">
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="82"/>
+    </row>
+    <row r="11" spans="2:15" s="46" customFormat="1" ht="220.5">
+      <c r="B11" s="83">
         <v>1</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="90"/>
-      <c r="E11" s="61" t="s">
+      <c r="D11" s="85"/>
+      <c r="E11" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="63">
+      <c r="G11" s="55">
         <v>3</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="55">
         <v>2.9</v>
       </c>
       <c r="I11" s="20">
@@ -4333,24 +4319,24 @@
         <v>24359999.999999996</v>
       </c>
       <c r="M11" s="17"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="49"/>
-    </row>
-    <row r="12" spans="2:15" s="47" customFormat="1" ht="15.6">
-      <c r="B12" s="89"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="61" t="s">
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
+    </row>
+    <row r="12" spans="2:15" s="46" customFormat="1" ht="15.75">
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="F12" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="63">
+      <c r="G12" s="55">
         <f>3+0.55*2</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="H12" s="63"/>
+      <c r="H12" s="55"/>
       <c r="I12" s="20">
         <v>1</v>
       </c>
@@ -4363,61 +4349,60 @@
         <v>1230000</v>
       </c>
       <c r="M12" s="17"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="49"/>
-    </row>
-    <row r="13" spans="2:15" s="68" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="72" t="s">
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
+    </row>
+    <row r="13" spans="2:15" s="12" customFormat="1" ht="15.6" customHeight="1">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="60"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="46">
+      <c r="J13" s="45">
         <f>SUM(J11:J12)</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="K13" s="44" t="s">
         <v>13</v>
       </c>
       <c r="L13" s="4">
         <f>SUM(L11:L12)</f>
         <v>25589999.999999996</v>
       </c>
-      <c r="M13" s="69"/>
-      <c r="N13" s="71"/>
-    </row>
-    <row r="14" spans="2:15" s="68" customFormat="1" ht="138.6" customHeight="1">
-      <c r="B14" s="112" t="s">
+      <c r="M13" s="14"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="2:15" s="12" customFormat="1" ht="138.6" customHeight="1">
+      <c r="B14" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="C14" s="113"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="71"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="L6:M6"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="B9:B10"/>
@@ -4428,13 +4413,14 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -4443,241 +4429,241 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="4.88671875" style="56" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="56" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" style="56" customWidth="1"/>
-    <col min="5" max="5" width="46.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="59" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="59" customWidth="1"/>
-    <col min="13" max="13" width="24.109375" style="56" customWidth="1"/>
-    <col min="14" max="14" width="19.109375" style="59" customWidth="1"/>
-    <col min="15" max="15" width="14.109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="4.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="112.5" customHeight="1">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="2:15" ht="49.5" customHeight="1">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-    </row>
-    <row r="3" spans="2:15" ht="13.95" customHeight="1">
-      <c r="B3" s="78" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+    </row>
+    <row r="3" spans="2:15" ht="13.9" customHeight="1">
+      <c r="B3" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-    </row>
-    <row r="6" spans="2:15" ht="16.8">
-      <c r="B6" s="110" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+    </row>
+    <row r="6" spans="2:15" ht="16.5">
+      <c r="B6" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="111" t="s">
+      <c r="L6" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="M6" s="111"/>
-    </row>
-    <row r="7" spans="2:15" ht="16.8">
-      <c r="B7" s="94" t="s">
+      <c r="M6" s="98"/>
+    </row>
+    <row r="7" spans="2:15" ht="16.5">
+      <c r="B7" s="87" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="59" t="s">
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L7" s="95" t="s">
+      <c r="L7" s="88" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="95"/>
+      <c r="M7" s="88"/>
     </row>
     <row r="8" spans="2:15" ht="33.6" customHeight="1">
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="87" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B9" s="102" t="s">
+      <c r="B9" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="106" t="s">
+      <c r="E9" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="108" t="s">
+      <c r="F9" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="104" t="s">
+      <c r="G9" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="105"/>
-      <c r="I9" s="96" t="s">
+      <c r="H9" s="96"/>
+      <c r="I9" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="96" t="s">
+      <c r="J9" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="96" t="s">
+      <c r="K9" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="98" t="s">
+      <c r="L9" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="100" t="s">
+      <c r="M9" s="81" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="30" customHeight="1">
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="109"/>
-      <c r="G10" s="58" t="s">
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="101"/>
-    </row>
-    <row r="11" spans="2:15" s="47" customFormat="1" ht="202.8">
-      <c r="B11" s="88">
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="82"/>
+    </row>
+    <row r="11" spans="2:15" s="46" customFormat="1" ht="220.5">
+      <c r="B11" s="83">
         <v>1</v>
       </c>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="90"/>
-      <c r="E11" s="61" t="s">
+      <c r="D11" s="85"/>
+      <c r="E11" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="63">
+      <c r="G11" s="55">
         <v>3</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="55">
         <v>2.9</v>
       </c>
       <c r="I11" s="20">
@@ -4695,24 +4681,24 @@
         <v>24359999.999999996</v>
       </c>
       <c r="M11" s="17"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="49"/>
-    </row>
-    <row r="12" spans="2:15" s="47" customFormat="1" ht="15.6">
-      <c r="B12" s="89"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="91"/>
-      <c r="E12" s="61" t="s">
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
+    </row>
+    <row r="12" spans="2:15" s="46" customFormat="1" ht="15.75">
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F12" s="62" t="s">
+      <c r="F12" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="63">
+      <c r="G12" s="55">
         <f>3+0.55*2</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="H12" s="63"/>
+      <c r="H12" s="55"/>
       <c r="I12" s="20">
         <v>1</v>
       </c>
@@ -4725,27 +4711,27 @@
         <v>1230000</v>
       </c>
       <c r="M12" s="17"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="49"/>
-    </row>
-    <row r="13" spans="2:15" s="47" customFormat="1" ht="78">
-      <c r="B13" s="88">
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
+    </row>
+    <row r="13" spans="2:15" s="46" customFormat="1" ht="78.75">
+      <c r="B13" s="83">
         <v>2</v>
       </c>
-      <c r="C13" s="88" t="s">
+      <c r="C13" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="61" t="s">
+      <c r="D13" s="85"/>
+      <c r="E13" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="55">
         <v>1.4</v>
       </c>
-      <c r="H13" s="63">
+      <c r="H13" s="55">
         <v>2.7</v>
       </c>
       <c r="I13" s="20">
@@ -4763,24 +4749,24 @@
         <v>15876000</v>
       </c>
       <c r="M13" s="17"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="49"/>
-    </row>
-    <row r="14" spans="2:15" s="47" customFormat="1" ht="15.6">
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="61" t="s">
+      <c r="N13" s="47"/>
+      <c r="O13" s="48"/>
+    </row>
+    <row r="14" spans="2:15" s="46" customFormat="1" ht="15.75">
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="63">
+      <c r="G14" s="55">
         <f>G13+0.55*2</f>
         <v>2.5</v>
       </c>
-      <c r="H14" s="63"/>
+      <c r="H14" s="55"/>
       <c r="I14" s="20">
         <v>2</v>
       </c>
@@ -4793,21 +4779,21 @@
         <v>1500000</v>
       </c>
       <c r="M14" s="17"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="49"/>
-    </row>
-    <row r="15" spans="2:15" s="47" customFormat="1" ht="109.2">
-      <c r="B15" s="89"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="61" t="s">
+      <c r="N14" s="47"/>
+      <c r="O14" s="48"/>
+    </row>
+    <row r="15" spans="2:15" s="46" customFormat="1" ht="110.25">
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="F15" s="62" t="s">
+      <c r="F15" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="20">
         <v>2</v>
       </c>
@@ -4820,27 +4806,27 @@
         <v>4500000</v>
       </c>
       <c r="M15" s="17"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="49"/>
-    </row>
-    <row r="16" spans="2:15" s="47" customFormat="1" ht="78">
-      <c r="B16" s="88">
+      <c r="N15" s="47"/>
+      <c r="O15" s="48"/>
+    </row>
+    <row r="16" spans="2:15" s="46" customFormat="1" ht="78.75">
+      <c r="B16" s="83">
         <v>3</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="90"/>
-      <c r="E16" s="61" t="s">
+      <c r="D16" s="85"/>
+      <c r="E16" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="63">
+      <c r="G16" s="55">
         <v>0.9</v>
       </c>
-      <c r="H16" s="63">
+      <c r="H16" s="55">
         <v>2.2000000000000002</v>
       </c>
       <c r="I16" s="20">
@@ -4858,21 +4844,21 @@
         <v>4158000</v>
       </c>
       <c r="M16" s="17"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="49"/>
-    </row>
-    <row r="17" spans="2:15" s="47" customFormat="1" ht="93.6">
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="61" t="s">
+      <c r="N16" s="47"/>
+      <c r="O16" s="48"/>
+    </row>
+    <row r="17" spans="2:15" s="46" customFormat="1" ht="94.5">
+      <c r="B17" s="84"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="53" t="s">
         <v>167</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="20">
         <v>1</v>
       </c>
@@ -4885,27 +4871,27 @@
         <v>1150000</v>
       </c>
       <c r="M17" s="17"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="49"/>
-    </row>
-    <row r="18" spans="2:15" s="47" customFormat="1" ht="78">
-      <c r="B18" s="88">
+      <c r="N17" s="47"/>
+      <c r="O17" s="48"/>
+    </row>
+    <row r="18" spans="2:15" s="46" customFormat="1" ht="78.75">
+      <c r="B18" s="83">
         <v>4</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="D18" s="90"/>
-      <c r="E18" s="61" t="s">
+      <c r="D18" s="85"/>
+      <c r="E18" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="63">
+      <c r="G18" s="55">
         <v>0.6</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="55">
         <v>1.65</v>
       </c>
       <c r="I18" s="20">
@@ -4923,21 +4909,21 @@
         <v>2079000</v>
       </c>
       <c r="M18" s="17"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="49"/>
-    </row>
-    <row r="19" spans="2:15" s="47" customFormat="1" ht="93.6">
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="61" t="s">
+      <c r="N18" s="47"/>
+      <c r="O18" s="48"/>
+    </row>
+    <row r="19" spans="2:15" s="46" customFormat="1" ht="94.5">
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="F19" s="62" t="s">
+      <c r="F19" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
       <c r="I19" s="20">
         <v>1</v>
       </c>
@@ -4950,27 +4936,27 @@
         <v>950000</v>
       </c>
       <c r="M19" s="17"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="49"/>
-    </row>
-    <row r="20" spans="2:15" s="47" customFormat="1" ht="78">
-      <c r="B20" s="88">
+      <c r="N19" s="47"/>
+      <c r="O19" s="48"/>
+    </row>
+    <row r="20" spans="2:15" s="46" customFormat="1" ht="78.75">
+      <c r="B20" s="83">
         <v>5</v>
       </c>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="90"/>
-      <c r="E20" s="61" t="s">
+      <c r="D20" s="85"/>
+      <c r="E20" s="53" t="s">
         <v>171</v>
       </c>
-      <c r="F20" s="62" t="s">
+      <c r="F20" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="63">
+      <c r="G20" s="55">
         <v>0.8</v>
       </c>
-      <c r="H20" s="63">
+      <c r="H20" s="55">
         <v>1.8</v>
       </c>
       <c r="I20" s="20">
@@ -4988,21 +4974,21 @@
         <v>5472000</v>
       </c>
       <c r="M20" s="17"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="49"/>
-    </row>
-    <row r="21" spans="2:15" s="47" customFormat="1" ht="78">
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="61" t="s">
+      <c r="N20" s="47"/>
+      <c r="O20" s="48"/>
+    </row>
+    <row r="21" spans="2:15" s="46" customFormat="1" ht="78.75">
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="F21" s="62" t="s">
+      <c r="F21" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
       <c r="I21" s="20">
         <v>2</v>
       </c>
@@ -5015,53 +5001,74 @@
         <v>900000</v>
       </c>
       <c r="M21" s="17"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="49"/>
-    </row>
-    <row r="22" spans="2:15" s="56" customFormat="1" ht="15.6" customHeight="1">
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="72" t="s">
+      <c r="N21" s="47"/>
+      <c r="O21" s="48"/>
+    </row>
+    <row r="22" spans="2:15" s="12" customFormat="1" ht="15.6" customHeight="1">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="60"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="46">
+      <c r="J22" s="45">
         <f>SUM(J11:J21)</f>
         <v>22.109999999999996</v>
       </c>
-      <c r="K22" s="45" t="s">
+      <c r="K22" s="44" t="s">
         <v>34</v>
       </c>
       <c r="L22" s="4">
         <f>SUM(L11:L21)</f>
         <v>62175000</v>
       </c>
-      <c r="M22" s="57"/>
-      <c r="N22" s="59"/>
-    </row>
-    <row r="23" spans="2:15" s="56" customFormat="1" ht="138.6" customHeight="1">
-      <c r="B23" s="112" t="s">
+      <c r="M22" s="14"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="2:15" s="12" customFormat="1" ht="138.6" customHeight="1">
+      <c r="B23" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="113"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="113"/>
-      <c r="J23" s="113"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="59"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
+      <c r="M23" s="76"/>
+      <c r="N23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="B23:M23"/>
     <mergeCell ref="E22:H22"/>
     <mergeCell ref="B1:M1"/>
@@ -5078,27 +5085,6 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0" bottom="0" header="0.5" footer="0.5"/>
   <pageSetup scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -5107,67 +5093,67 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="8.6640625" style="24"/>
-    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="24"/>
-    <col min="8" max="8" width="13.33203125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" style="24"/>
-    <col min="10" max="10" width="14.33203125" style="24" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="24" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" style="24" customWidth="1"/>
+    <col min="1" max="3" width="8.7109375" style="24"/>
+    <col min="4" max="4" width="9.7109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="24"/>
+    <col min="8" max="8" width="13.28515625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="24"/>
+    <col min="10" max="10" width="14.28515625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="24" customWidth="1"/>
     <col min="15" max="15" width="11" style="24" customWidth="1"/>
-    <col min="16" max="16" width="14.5546875" style="24" customWidth="1"/>
-    <col min="17" max="16384" width="8.6640625" style="24"/>
+    <col min="16" max="16" width="14.5703125" style="24" customWidth="1"/>
+    <col min="17" max="16384" width="8.7109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23.4">
-      <c r="B1" s="140" t="s">
+    <row r="1" spans="1:17" ht="23.25">
+      <c r="B1" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="140"/>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
-      <c r="N1" s="140"/>
-      <c r="O1" s="140"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
+      <c r="M1" s="101"/>
+      <c r="N1" s="101"/>
+      <c r="O1" s="101"/>
       <c r="P1" s="25"/>
       <c r="Q1" s="25"/>
     </row>
-    <row r="2" spans="1:17" ht="23.4">
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
+    <row r="2" spans="1:17" ht="23.25">
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
     </row>
@@ -5183,46 +5169,46 @@
       <c r="K5" s="27"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="141"/>
-      <c r="C6" s="141" t="s">
+      <c r="B6" s="102"/>
+      <c r="C6" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="142" t="s">
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="142"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="142"/>
-      <c r="J6" s="143" t="s">
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="K6" s="143"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="144" t="s">
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="146" t="s">
+      <c r="O6" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="P6" s="134" t="s">
+      <c r="P6" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="Q6" s="134" t="s">
+      <c r="Q6" s="113" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="141"/>
-      <c r="B7" s="141"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
+      <c r="A7" s="102"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
       <c r="F7" s="28" t="s">
         <v>91</v>
       </c>
@@ -5245,19 +5231,19 @@
       <c r="M7" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="N7" s="145"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
+      <c r="N7" s="106"/>
+      <c r="O7" s="108"/>
+      <c r="P7" s="114"/>
+      <c r="Q7" s="114"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="125"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="126" t="s">
+      <c r="A8" s="109"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="115" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="115"/>
       <c r="F8" s="30" t="e">
         <f>H8/G8</f>
         <v>#REF!</v>
@@ -5298,11 +5284,11 @@
       <c r="Q8" s="30"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="125"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
+      <c r="A9" s="109"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30">
@@ -5326,13 +5312,13 @@
       <c r="Q9" s="30"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="125"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="131" t="s">
+      <c r="A10" s="109"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="110" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="132"/>
-      <c r="E10" s="133"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="112"/>
       <c r="F10" s="30">
         <v>1900000</v>
       </c>
@@ -5360,20 +5346,20 @@
       <c r="Q10" s="30"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="125"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="131" t="s">
+      <c r="A11" s="109"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="110" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="132"/>
-      <c r="E11" s="133"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="112"/>
       <c r="F11" s="30">
         <v>180000</v>
       </c>
       <c r="G11" s="30">
         <v>7</v>
       </c>
-      <c r="H11" s="50"/>
+      <c r="H11" s="49"/>
       <c r="I11" s="30"/>
       <c r="J11" s="30">
         <f>F11*G11</f>
@@ -5394,17 +5380,17 @@
       <c r="Q11" s="30"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="125"/>
-      <c r="B12" s="125"/>
-      <c r="C12" s="137" t="s">
+      <c r="A12" s="109"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="110" t="s">
         <v>147</v>
       </c>
-      <c r="D12" s="138"/>
-      <c r="E12" s="139"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="112"/>
       <c r="F12" s="30">
         <v>230000</v>
       </c>
-      <c r="G12" s="60">
+      <c r="G12" s="52">
         <f>G8</f>
         <v>22.109999999999996</v>
       </c>
@@ -5429,17 +5415,17 @@
       <c r="Q12" s="30"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="125"/>
-      <c r="B13" s="125"/>
-      <c r="C13" s="131" t="s">
+      <c r="A13" s="109"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="132"/>
-      <c r="E13" s="133"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="112"/>
       <c r="F13" s="30">
         <v>150000</v>
       </c>
-      <c r="G13" s="60">
+      <c r="G13" s="52">
         <f>G8</f>
         <v>22.109999999999996</v>
       </c>
@@ -5464,11 +5450,11 @@
       <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="125"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="133"/>
+      <c r="A14" s="109"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
@@ -5489,11 +5475,11 @@
       <c r="Q14" s="30"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="125"/>
-      <c r="B15" s="125"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="132"/>
-      <c r="E15" s="133"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="112"/>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
@@ -5514,11 +5500,11 @@
       <c r="Q15" s="30"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="125"/>
-      <c r="B16" s="125"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="112"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -5539,11 +5525,11 @@
       <c r="Q16" s="30"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="125"/>
-      <c r="B17" s="125"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30">
@@ -5567,11 +5553,11 @@
       <c r="Q17" s="30"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="125"/>
-      <c r="B18" s="125"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30">
@@ -5595,11 +5581,11 @@
       <c r="Q18" s="30"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="125"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="30">
@@ -5623,11 +5609,11 @@
       <c r="Q19" s="30"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="125"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
       <c r="H20" s="30" t="e">
@@ -5669,7 +5655,7 @@
       <c r="H21" s="33"/>
       <c r="J21" s="34"/>
     </row>
-    <row r="22" spans="1:17" ht="33.6">
+    <row r="22" spans="1:17" ht="33.75">
       <c r="A22" s="24" t="s">
         <v>7</v>
       </c>
@@ -5683,7 +5669,7 @@
       </c>
       <c r="Q22" s="35"/>
     </row>
-    <row r="23" spans="1:17" ht="23.4">
+    <row r="23" spans="1:17" ht="23.25">
       <c r="B23" s="24" t="s">
         <v>99</v>
       </c>
@@ -5709,30 +5695,30 @@
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="C27" s="126" t="s">
+      <c r="C27" s="115" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="126"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="126"/>
-      <c r="H27" s="126"/>
-      <c r="I27" s="126"/>
-      <c r="J27" s="126"/>
-      <c r="K27" s="126"/>
-      <c r="L27" s="126"/>
-      <c r="M27" s="126"/>
-      <c r="N27" s="126"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="115"/>
+      <c r="L27" s="115"/>
+      <c r="M27" s="115"/>
+      <c r="N27" s="115"/>
     </row>
     <row r="28" spans="1:17" ht="45" customHeight="1">
       <c r="B28" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="127" t="s">
+      <c r="C28" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="127"/>
-      <c r="E28" s="128"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="118"/>
       <c r="F28" s="38" t="s">
         <v>106</v>
       </c>
@@ -5740,373 +5726,373 @@
       <c r="H28" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="I28" s="129" t="s">
+      <c r="I28" s="119" t="s">
         <v>108</v>
       </c>
-      <c r="J28" s="130"/>
-      <c r="K28" s="129" t="s">
+      <c r="J28" s="120"/>
+      <c r="K28" s="119" t="s">
         <v>109</v>
       </c>
-      <c r="L28" s="130"/>
-      <c r="M28" s="129" t="s">
+      <c r="L28" s="120"/>
+      <c r="M28" s="119" t="s">
         <v>110</v>
       </c>
-      <c r="N28" s="130"/>
-    </row>
-    <row r="29" spans="1:17" ht="18">
-      <c r="B29" s="117">
+      <c r="N28" s="120"/>
+    </row>
+    <row r="29" spans="1:17" ht="18.75">
+      <c r="B29" s="121">
         <v>1</v>
       </c>
-      <c r="C29" s="121" t="s">
+      <c r="C29" s="124" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="115" t="s">
+      <c r="D29" s="124"/>
+      <c r="E29" s="125"/>
+      <c r="F29" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G29" s="115"/>
-      <c r="H29" s="116">
+      <c r="G29" s="126"/>
+      <c r="H29" s="129">
         <v>0.5</v>
       </c>
-      <c r="I29" s="123">
+      <c r="I29" s="127">
         <v>100000000</v>
       </c>
-      <c r="J29" s="123"/>
-      <c r="K29" s="124">
+      <c r="J29" s="127"/>
+      <c r="K29" s="128">
         <f>H29*I29</f>
         <v>50000000</v>
       </c>
-      <c r="L29" s="116"/>
-      <c r="M29" s="124">
+      <c r="L29" s="129"/>
+      <c r="M29" s="128">
         <f>M27*K29</f>
         <v>0</v>
       </c>
-      <c r="N29" s="116"/>
-    </row>
-    <row r="30" spans="1:17" ht="18">
-      <c r="B30" s="118"/>
-      <c r="C30" s="121"/>
-      <c r="D30" s="121"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="115" t="s">
+      <c r="N29" s="129"/>
+    </row>
+    <row r="30" spans="1:17" ht="18.75">
+      <c r="B30" s="122"/>
+      <c r="C30" s="124"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="125"/>
+      <c r="F30" s="126" t="s">
         <v>113</v>
       </c>
-      <c r="G30" s="115"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="116"/>
-    </row>
-    <row r="31" spans="1:17" ht="18">
-      <c r="B31" s="119"/>
-      <c r="C31" s="121"/>
-      <c r="D31" s="121"/>
-      <c r="E31" s="122"/>
-      <c r="F31" s="115" t="s">
+      <c r="G30" s="126"/>
+      <c r="H30" s="129"/>
+      <c r="I30" s="129"/>
+      <c r="J30" s="129"/>
+      <c r="K30" s="129"/>
+      <c r="L30" s="129"/>
+      <c r="M30" s="129"/>
+      <c r="N30" s="129"/>
+    </row>
+    <row r="31" spans="1:17" ht="18.75">
+      <c r="B31" s="123"/>
+      <c r="C31" s="124"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="125"/>
+      <c r="F31" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G31" s="115"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="116"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
-    </row>
-    <row r="32" spans="1:17" ht="18">
-      <c r="B32" s="117">
+      <c r="G31" s="126"/>
+      <c r="H31" s="129"/>
+      <c r="I31" s="129"/>
+      <c r="J31" s="129"/>
+      <c r="K31" s="129"/>
+      <c r="L31" s="129"/>
+      <c r="M31" s="129"/>
+      <c r="N31" s="129"/>
+    </row>
+    <row r="32" spans="1:17" ht="18.75">
+      <c r="B32" s="121">
         <v>2</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="124" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="122"/>
-      <c r="F32" s="115" t="s">
+      <c r="D32" s="124"/>
+      <c r="E32" s="125"/>
+      <c r="F32" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="115"/>
-      <c r="H32" s="117">
+      <c r="G32" s="126"/>
+      <c r="H32" s="121">
         <v>0.8</v>
       </c>
-      <c r="I32" s="123">
+      <c r="I32" s="127">
         <v>2500000</v>
       </c>
-      <c r="J32" s="123"/>
-      <c r="K32" s="124">
+      <c r="J32" s="127"/>
+      <c r="K32" s="128">
         <f>0.5*I32</f>
         <v>1250000</v>
       </c>
-      <c r="L32" s="116"/>
-      <c r="M32" s="124"/>
-      <c r="N32" s="116"/>
-    </row>
-    <row r="33" spans="2:14" ht="18">
-      <c r="B33" s="118"/>
-      <c r="C33" s="121"/>
-      <c r="D33" s="121"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="115" t="s">
+      <c r="L32" s="129"/>
+      <c r="M32" s="128"/>
+      <c r="N32" s="129"/>
+    </row>
+    <row r="33" spans="2:14" ht="18.75">
+      <c r="B33" s="122"/>
+      <c r="C33" s="124"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="125"/>
+      <c r="F33" s="126" t="s">
         <v>115</v>
       </c>
-      <c r="G33" s="115"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="116"/>
-      <c r="N33" s="116"/>
-    </row>
-    <row r="34" spans="2:14" ht="18">
-      <c r="B34" s="119"/>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="122"/>
-      <c r="F34" s="115" t="s">
+      <c r="G33" s="126"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="129"/>
+      <c r="J33" s="129"/>
+      <c r="K33" s="129"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
+    </row>
+    <row r="34" spans="2:14" ht="18.75">
+      <c r="B34" s="123"/>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="125"/>
+      <c r="F34" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G34" s="115"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
-    </row>
-    <row r="35" spans="2:14" ht="18">
-      <c r="B35" s="117">
+      <c r="G34" s="126"/>
+      <c r="H34" s="122"/>
+      <c r="I34" s="129"/>
+      <c r="J34" s="129"/>
+      <c r="K34" s="129"/>
+      <c r="L34" s="129"/>
+      <c r="M34" s="129"/>
+      <c r="N34" s="129"/>
+    </row>
+    <row r="35" spans="2:14" ht="18.75">
+      <c r="B35" s="121">
         <v>3</v>
       </c>
-      <c r="C35" s="121" t="s">
+      <c r="C35" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="D35" s="121"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="115" t="s">
+      <c r="D35" s="124"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G35" s="115"/>
-      <c r="H35" s="116">
+      <c r="G35" s="126"/>
+      <c r="H35" s="129">
         <v>1</v>
       </c>
-      <c r="I35" s="116"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="116"/>
-      <c r="L35" s="116"/>
-      <c r="M35" s="116"/>
-      <c r="N35" s="116"/>
-    </row>
-    <row r="36" spans="2:14" ht="18">
-      <c r="B36" s="118"/>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="115" t="s">
+      <c r="I35" s="129"/>
+      <c r="J35" s="129"/>
+      <c r="K35" s="129"/>
+      <c r="L35" s="129"/>
+      <c r="M35" s="129"/>
+      <c r="N35" s="129"/>
+    </row>
+    <row r="36" spans="2:14" ht="18.75">
+      <c r="B36" s="122"/>
+      <c r="C36" s="124"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="125"/>
+      <c r="F36" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="115"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="116"/>
-      <c r="K36" s="116"/>
-      <c r="L36" s="116"/>
-      <c r="M36" s="116"/>
-      <c r="N36" s="116"/>
-    </row>
-    <row r="37" spans="2:14" ht="18">
-      <c r="B37" s="119"/>
-      <c r="C37" s="121"/>
-      <c r="D37" s="121"/>
-      <c r="E37" s="122"/>
-      <c r="F37" s="115" t="s">
+      <c r="G36" s="126"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="129"/>
+      <c r="K36" s="129"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="129"/>
+      <c r="N36" s="129"/>
+    </row>
+    <row r="37" spans="2:14" ht="18.75">
+      <c r="B37" s="123"/>
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="125"/>
+      <c r="F37" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G37" s="115"/>
-      <c r="H37" s="116"/>
-      <c r="I37" s="116"/>
-      <c r="J37" s="116"/>
-      <c r="K37" s="116"/>
-      <c r="L37" s="116"/>
-      <c r="M37" s="116"/>
-      <c r="N37" s="116"/>
-    </row>
-    <row r="38" spans="2:14" ht="18">
-      <c r="B38" s="117">
+      <c r="G37" s="126"/>
+      <c r="H37" s="129"/>
+      <c r="I37" s="129"/>
+      <c r="J37" s="129"/>
+      <c r="K37" s="129"/>
+      <c r="L37" s="129"/>
+      <c r="M37" s="129"/>
+      <c r="N37" s="129"/>
+    </row>
+    <row r="38" spans="2:14" ht="18.75">
+      <c r="B38" s="121">
         <v>4</v>
       </c>
-      <c r="C38" s="121" t="s">
+      <c r="C38" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="121"/>
-      <c r="E38" s="122"/>
-      <c r="F38" s="115" t="s">
+      <c r="D38" s="124"/>
+      <c r="E38" s="125"/>
+      <c r="F38" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="G38" s="115"/>
-      <c r="H38" s="116">
+      <c r="G38" s="126"/>
+      <c r="H38" s="129">
         <v>1.2</v>
       </c>
-      <c r="I38" s="116"/>
-      <c r="J38" s="116"/>
-      <c r="K38" s="116"/>
-      <c r="L38" s="116"/>
-      <c r="M38" s="116"/>
-      <c r="N38" s="116"/>
-    </row>
-    <row r="39" spans="2:14" ht="18">
-      <c r="B39" s="118"/>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="115" t="s">
+      <c r="I38" s="129"/>
+      <c r="J38" s="129"/>
+      <c r="K38" s="129"/>
+      <c r="L38" s="129"/>
+      <c r="M38" s="129"/>
+      <c r="N38" s="129"/>
+    </row>
+    <row r="39" spans="2:14" ht="18.75">
+      <c r="B39" s="122"/>
+      <c r="C39" s="124"/>
+      <c r="D39" s="124"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G39" s="115"/>
-      <c r="H39" s="116"/>
-      <c r="I39" s="116"/>
-      <c r="J39" s="116"/>
-      <c r="K39" s="116"/>
-      <c r="L39" s="116"/>
-      <c r="M39" s="116"/>
-      <c r="N39" s="116"/>
-    </row>
-    <row r="40" spans="2:14" ht="18">
-      <c r="B40" s="119"/>
-      <c r="C40" s="121"/>
-      <c r="D40" s="121"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="115" t="s">
+      <c r="G39" s="126"/>
+      <c r="H39" s="129"/>
+      <c r="I39" s="129"/>
+      <c r="J39" s="129"/>
+      <c r="K39" s="129"/>
+      <c r="L39" s="129"/>
+      <c r="M39" s="129"/>
+      <c r="N39" s="129"/>
+    </row>
+    <row r="40" spans="2:14" ht="18.75">
+      <c r="B40" s="123"/>
+      <c r="C40" s="124"/>
+      <c r="D40" s="124"/>
+      <c r="E40" s="125"/>
+      <c r="F40" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G40" s="115"/>
-      <c r="H40" s="116"/>
-      <c r="I40" s="116"/>
-      <c r="J40" s="116"/>
-      <c r="K40" s="116"/>
-      <c r="L40" s="116"/>
-      <c r="M40" s="116"/>
-      <c r="N40" s="116"/>
-    </row>
-    <row r="41" spans="2:14" ht="18">
-      <c r="B41" s="117">
+      <c r="G40" s="126"/>
+      <c r="H40" s="129"/>
+      <c r="I40" s="129"/>
+      <c r="J40" s="129"/>
+      <c r="K40" s="129"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="129"/>
+      <c r="N40" s="129"/>
+    </row>
+    <row r="41" spans="2:14" ht="18.75">
+      <c r="B41" s="121">
         <v>5</v>
       </c>
-      <c r="C41" s="121" t="s">
+      <c r="C41" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="121"/>
-      <c r="E41" s="122"/>
-      <c r="F41" s="115" t="s">
+      <c r="D41" s="124"/>
+      <c r="E41" s="125"/>
+      <c r="F41" s="126" t="s">
         <v>119</v>
       </c>
-      <c r="G41" s="115"/>
-      <c r="H41" s="116">
+      <c r="G41" s="126"/>
+      <c r="H41" s="129">
         <v>1.5</v>
       </c>
-      <c r="I41" s="116"/>
-      <c r="J41" s="116"/>
-      <c r="K41" s="116"/>
-      <c r="L41" s="116"/>
-      <c r="M41" s="116"/>
-      <c r="N41" s="116"/>
-    </row>
-    <row r="42" spans="2:14" ht="18">
-      <c r="B42" s="118"/>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="115" t="s">
+      <c r="I41" s="129"/>
+      <c r="J41" s="129"/>
+      <c r="K41" s="129"/>
+      <c r="L41" s="129"/>
+      <c r="M41" s="129"/>
+      <c r="N41" s="129"/>
+    </row>
+    <row r="42" spans="2:14" ht="18.75">
+      <c r="B42" s="122"/>
+      <c r="C42" s="124"/>
+      <c r="D42" s="124"/>
+      <c r="E42" s="125"/>
+      <c r="F42" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G42" s="115"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="116"/>
-      <c r="L42" s="116"/>
-      <c r="M42" s="116"/>
-      <c r="N42" s="116"/>
-    </row>
-    <row r="43" spans="2:14" ht="18">
-      <c r="B43" s="119"/>
-      <c r="C43" s="121"/>
-      <c r="D43" s="121"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="115" t="s">
+      <c r="G42" s="126"/>
+      <c r="H42" s="129"/>
+      <c r="I42" s="129"/>
+      <c r="J42" s="129"/>
+      <c r="K42" s="129"/>
+      <c r="L42" s="129"/>
+      <c r="M42" s="129"/>
+      <c r="N42" s="129"/>
+    </row>
+    <row r="43" spans="2:14" ht="18.75">
+      <c r="B43" s="123"/>
+      <c r="C43" s="124"/>
+      <c r="D43" s="124"/>
+      <c r="E43" s="125"/>
+      <c r="F43" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G43" s="115"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="116"/>
-      <c r="L43" s="116"/>
-      <c r="M43" s="116"/>
-      <c r="N43" s="116"/>
-    </row>
-    <row r="44" spans="2:14" ht="18">
-      <c r="B44" s="117">
+      <c r="G43" s="126"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="129"/>
+      <c r="K43" s="129"/>
+      <c r="L43" s="129"/>
+      <c r="M43" s="129"/>
+      <c r="N43" s="129"/>
+    </row>
+    <row r="44" spans="2:14" ht="18.75">
+      <c r="B44" s="121">
         <v>6</v>
       </c>
-      <c r="C44" s="120" t="s">
+      <c r="C44" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="115" t="s">
+      <c r="D44" s="130"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G44" s="115"/>
-      <c r="H44" s="116">
+      <c r="G44" s="126"/>
+      <c r="H44" s="129">
         <v>0</v>
       </c>
-      <c r="I44" s="116"/>
-      <c r="J44" s="116"/>
-      <c r="K44" s="116"/>
-      <c r="L44" s="116"/>
-      <c r="M44" s="116"/>
-      <c r="N44" s="116"/>
-    </row>
-    <row r="45" spans="2:14" ht="18">
-      <c r="B45" s="118"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="115" t="s">
+      <c r="I44" s="129"/>
+      <c r="J44" s="129"/>
+      <c r="K44" s="129"/>
+      <c r="L44" s="129"/>
+      <c r="M44" s="129"/>
+      <c r="N44" s="129"/>
+    </row>
+    <row r="45" spans="2:14" ht="18.75">
+      <c r="B45" s="122"/>
+      <c r="C45" s="130"/>
+      <c r="D45" s="130"/>
+      <c r="E45" s="130"/>
+      <c r="F45" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="115"/>
-      <c r="H45" s="116"/>
-      <c r="I45" s="116"/>
-      <c r="J45" s="116"/>
-      <c r="K45" s="116"/>
-      <c r="L45" s="116"/>
-      <c r="M45" s="116"/>
-      <c r="N45" s="116"/>
-    </row>
-    <row r="46" spans="2:14" ht="18">
-      <c r="B46" s="119"/>
-      <c r="C46" s="120"/>
-      <c r="D46" s="120"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="115" t="s">
+      <c r="G45" s="126"/>
+      <c r="H45" s="129"/>
+      <c r="I45" s="129"/>
+      <c r="J45" s="129"/>
+      <c r="K45" s="129"/>
+      <c r="L45" s="129"/>
+      <c r="M45" s="129"/>
+      <c r="N45" s="129"/>
+    </row>
+    <row r="46" spans="2:14" ht="18.75">
+      <c r="B46" s="123"/>
+      <c r="C46" s="130"/>
+      <c r="D46" s="130"/>
+      <c r="E46" s="130"/>
+      <c r="F46" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="G46" s="115"/>
-      <c r="H46" s="116"/>
-      <c r="I46" s="116"/>
-      <c r="J46" s="116"/>
-      <c r="K46" s="116"/>
-      <c r="L46" s="116"/>
-      <c r="M46" s="116"/>
-      <c r="N46" s="116"/>
+      <c r="G46" s="126"/>
+      <c r="H46" s="129"/>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129"/>
+      <c r="K46" s="129"/>
+      <c r="L46" s="129"/>
+      <c r="M46" s="129"/>
+      <c r="N46" s="129"/>
     </row>
     <row r="48" spans="2:14">
       <c r="C48" s="24" t="s">
@@ -6125,42 +6111,72 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="B1:O2"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:E7"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C27:N27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:E46"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:E43"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:E40"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:E37"/>
+    <mergeCell ref="F35:G35"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:E34"/>
     <mergeCell ref="F32:G32"/>
@@ -6185,72 +6201,42 @@
     <mergeCell ref="M32:N32"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:E40"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:E37"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:E43"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="K41:L41"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:E46"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C27:N27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E9"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B1:O2"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:E7"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6258,7 +6244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6268,25 +6254,25 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:8" ht="72.599999999999994" customHeight="1">
-      <c r="B6" s="148" t="s">
+      <c r="B6" s="131" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="149"/>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
-      <c r="H6" s="149"/>
-    </row>
-    <row r="7" spans="2:8" ht="28.8">
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+    </row>
+    <row r="7" spans="2:8" ht="30">
       <c r="B7" s="40" t="s">
         <v>8</v>
       </c>
@@ -6309,260 +6295,260 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B8" s="51">
+    <row r="8" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="16">
         <v>500</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="16">
         <v>2493</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="16">
         <v>2</v>
       </c>
-      <c r="H8" s="151" t="s">
+      <c r="H8" s="134" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B9" s="53">
+    <row r="9" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B9" s="16">
         <v>2</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="16">
         <v>500</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="16">
         <v>2470</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="H9" s="152"/>
-    </row>
-    <row r="10" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B10" s="53">
+      <c r="H9" s="135"/>
+    </row>
+    <row r="10" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B10" s="16">
         <v>3</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="16">
         <v>525</v>
       </c>
-      <c r="F10" s="53">
+      <c r="F10" s="16">
         <v>1478</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="16">
         <v>2</v>
       </c>
-      <c r="H10" s="152"/>
-    </row>
-    <row r="11" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B11" s="53">
+      <c r="H10" s="135"/>
+    </row>
+    <row r="11" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B11" s="16">
         <v>4</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="16">
         <v>525</v>
       </c>
-      <c r="F11" s="53">
+      <c r="F11" s="16">
         <v>1480</v>
       </c>
-      <c r="G11" s="53">
+      <c r="G11" s="16">
         <v>2</v>
       </c>
-      <c r="H11" s="152"/>
-    </row>
-    <row r="12" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B12" s="53">
+      <c r="H11" s="135"/>
+    </row>
+    <row r="12" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B12" s="16">
         <v>5</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="51" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="16">
         <v>398</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="16">
         <v>1203</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="16">
         <v>2</v>
       </c>
-      <c r="H12" s="152"/>
-    </row>
-    <row r="13" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B13" s="53">
+      <c r="H12" s="135"/>
+    </row>
+    <row r="13" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B13" s="16">
         <v>6</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="16">
         <v>398</v>
       </c>
-      <c r="F13" s="53">
+      <c r="F13" s="16">
         <v>1205</v>
       </c>
-      <c r="G13" s="53">
+      <c r="G13" s="16">
         <v>2</v>
       </c>
-      <c r="H13" s="153"/>
-    </row>
-    <row r="14" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B14" s="54">
+      <c r="H13" s="136"/>
+    </row>
+    <row r="14" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B14" s="16">
         <v>1</v>
       </c>
-      <c r="C14" s="154" t="s">
+      <c r="C14" s="137" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="137" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="16">
         <v>693</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="16">
         <v>2151</v>
       </c>
-      <c r="G14" s="54">
+      <c r="G14" s="16">
         <v>2</v>
       </c>
-      <c r="H14" s="151" t="s">
+      <c r="H14" s="134" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B15" s="54">
+    <row r="15" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B15" s="16">
         <v>2</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="155"/>
-      <c r="E15" s="54">
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="16">
         <v>618</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="16">
         <v>2151</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="16">
         <v>2</v>
       </c>
-      <c r="H15" s="152"/>
-    </row>
-    <row r="16" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B16" s="54">
+      <c r="H15" s="135"/>
+    </row>
+    <row r="16" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B16" s="16">
         <v>3</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="155"/>
-      <c r="E16" s="54">
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="16">
         <v>340</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="16">
         <v>708</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="16">
         <v>2</v>
       </c>
-      <c r="H16" s="152"/>
-    </row>
-    <row r="17" spans="2:8" ht="31.2" hidden="1" customHeight="1">
-      <c r="B17" s="54">
+      <c r="H16" s="135"/>
+    </row>
+    <row r="17" spans="2:8" ht="31.15" hidden="1" customHeight="1">
+      <c r="B17" s="16">
         <v>4</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="156"/>
-      <c r="E17" s="64">
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="16">
         <v>340</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="16">
         <v>1571</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="16">
         <v>1</v>
       </c>
-      <c r="H17" s="153"/>
-    </row>
-    <row r="18" spans="2:8" ht="31.2" customHeight="1">
-      <c r="B18" s="65">
+      <c r="H17" s="136"/>
+    </row>
+    <row r="18" spans="2:8" ht="31.15" customHeight="1">
+      <c r="B18" s="16">
         <v>1</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="65">
+      <c r="E18" s="16">
         <v>714</v>
       </c>
-      <c r="F18" s="65">
+      <c r="F18" s="16">
         <v>1825</v>
       </c>
-      <c r="G18" s="65">
+      <c r="G18" s="16">
         <v>1</v>
       </c>
-      <c r="H18" s="151" t="s">
+      <c r="H18" s="134" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="31.2" customHeight="1">
-      <c r="B19" s="65">
+    <row r="19" spans="2:8" ht="31.15" customHeight="1">
+      <c r="B19" s="16">
         <v>2</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="D19" s="67" t="s">
+      <c r="D19" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="65">
+      <c r="E19" s="16">
         <v>577</v>
       </c>
-      <c r="F19" s="65">
+      <c r="F19" s="16">
         <v>1942</v>
       </c>
-      <c r="G19" s="65">
+      <c r="G19" s="16">
         <v>1</v>
       </c>
-      <c r="H19" s="153"/>
+      <c r="H19" s="136"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="150" t="s">
+      <c r="B20" s="133" t="s">
         <v>133</v>
       </c>
-      <c r="C20" s="150"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
+      <c r="C20" s="133"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
       <c r="G20" s="42">
         <f>SUM(G18:G19)</f>
         <v>2</v>

</xml_diff>